<commit_message>
[ADD] Proceso 1 done
</commit_message>
<xml_diff>
--- a/Proyecto/Venta/clientes-varios/clientes-departamentales/clientes-departamentales.xlsx
+++ b/Proyecto/Venta/clientes-varios/clientes-departamentales/clientes-departamentales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josem\OneDrive\Documentos\UiPath\Venta\clientes-varios\clientes-departamentales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMEN\Documents\Gerenciales2\SOG21S25_201709282\Proyecto\Venta\clientes-varios\clientes-departamentales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26382AC3-E581-4751-B7B1-14C8E2EECED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEC82C5-E5E2-4FB9-B3F5-1B63225A1F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -908,7 +908,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -932,7 +932,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A51" si="0">A3+1</f>
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -956,7 +956,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1004,7 +1004,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1028,7 +1028,7 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1052,7 +1052,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1076,7 +1076,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1100,7 +1100,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -1124,7 +1124,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
@@ -1148,7 +1148,7 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1172,7 +1172,7 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1196,7 +1196,7 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
@@ -1220,7 +1220,7 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>53</v>
@@ -1244,7 +1244,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
         <v>57</v>
@@ -1268,7 +1268,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>60</v>
@@ -1292,7 +1292,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
@@ -1316,7 +1316,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
@@ -1340,7 +1340,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
         <v>71</v>
@@ -1364,7 +1364,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -1388,7 +1388,7 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
@@ -1412,7 +1412,7 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1436,7 +1436,7 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
         <v>83</v>
@@ -1460,7 +1460,7 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>86</v>
@@ -1484,7 +1484,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
@@ -1508,7 +1508,7 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
@@ -1532,7 +1532,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
@@ -1556,7 +1556,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
         <v>98</v>
@@ -1580,7 +1580,7 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
@@ -1604,7 +1604,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>103</v>
@@ -1628,7 +1628,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>107</v>
@@ -1652,7 +1652,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
@@ -1676,7 +1676,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>77</v>
@@ -1700,7 +1700,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>115</v>
@@ -1724,7 +1724,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>119</v>
@@ -1748,7 +1748,7 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>122</v>
@@ -1772,7 +1772,7 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
         <v>125</v>
@@ -1796,7 +1796,7 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>128</v>
@@ -1820,7 +1820,7 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
         <v>130</v>
@@ -1844,7 +1844,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>132</v>
@@ -1868,7 +1868,7 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
         <v>135</v>
@@ -1892,7 +1892,7 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
         <v>71</v>
@@ -1916,7 +1916,7 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
         <v>95</v>
@@ -1940,7 +1940,7 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -1964,7 +1964,7 @@
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
         <v>144</v>
@@ -1988,7 +1988,7 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
         <v>146</v>
@@ -2012,7 +2012,7 @@
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>83</v>
@@ -2036,7 +2036,7 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
         <v>152</v>
@@ -2060,7 +2060,7 @@
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
         <v>155</v>

</xml_diff>